<commit_message>
Generated PDF report layouts are now all fixed. Fertilization Recommendations to be added.
</commit_message>
<xml_diff>
--- a/Test Reports/2478_test.xlsx
+++ b/Test Reports/2478_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,423 +424,178 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>Test ID</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Test ID</t>
+          <t>Collection Date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Sample Collection Date</t>
+          <t>Latitude</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Latitude</t>
+          <t>Longitude</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Longitude</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Area (ha)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Area (ha)</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Address</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Mobile No.</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Mobile No.</t>
+          <t>Soil pH</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>Soil pH</t>
+          <t>Nitrogen</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Nitrogen</t>
+          <t>Phosphorus</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>Phosphorus</t>
+          <t>Potassium</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Potassium</t>
+          <t>Electrical Conductivity</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Electrical Conductivity</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>Moisture</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Moisture</t>
+          <t>Humidity</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Humidity</t>
+          <t>Soil Health Score</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>Soil Health Score</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Crop Recommendations</t>
+          <t>Recommendations</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>174</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2478</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2478</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>18-03-2024</t>
-        </is>
+          <t>16-04-2024</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>365</v>
       </c>
       <c r="D2" t="n">
-        <v>256</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2633</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>sdjhajksd</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="inlineStr">
+        <v>254</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>asuhgdjhasdkjajksdh ahsdjhajkshd jk asj</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>41</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="H2" t="n">
+        <v>45</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>231321</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2313213221</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" t="n">
+        <v>233</v>
+      </c>
+      <c r="M2" t="n">
         <v>26</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>9865362326</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>7</v>
-      </c>
-      <c r="M2" t="n">
-        <v>250</v>
-      </c>
       <c r="N2" t="n">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="O2" t="n">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" t="n">
-        <v>24</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.5293186647539065</v>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>175</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2478</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>18-03-2024</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>256</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2633</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>sdjhajksd</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>6</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>26</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>9865362326</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>7</v>
-      </c>
-      <c r="M3" t="n">
-        <v>250</v>
-      </c>
-      <c r="N3" t="n">
-        <v>100</v>
-      </c>
-      <c r="O3" t="n">
-        <v>120</v>
-      </c>
-      <c r="P3" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>25</v>
-      </c>
-      <c r="R3" t="n">
-        <v>33</v>
-      </c>
-      <c r="S3" t="n">
-        <v>24</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.5293186647539065</v>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>176</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2478</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>18-03-2024</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>256</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2633</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>sdjhajksd</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>26</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>9865362326</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>7</v>
-      </c>
-      <c r="M4" t="n">
-        <v>250</v>
-      </c>
-      <c r="N4" t="n">
-        <v>100</v>
-      </c>
-      <c r="O4" t="n">
-        <v>120</v>
-      </c>
-      <c r="P4" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>25</v>
-      </c>
-      <c r="R4" t="n">
-        <v>33</v>
-      </c>
-      <c r="S4" t="n">
-        <v>24</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.5293186647539065</v>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>177</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2478</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>18-03-2024</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>256</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2633</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>sdjhajksd</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>6</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>26</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>9865362326</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>7</v>
-      </c>
-      <c r="M5" t="n">
-        <v>250</v>
-      </c>
-      <c r="N5" t="n">
-        <v>100</v>
-      </c>
-      <c r="O5" t="n">
-        <v>120</v>
-      </c>
-      <c r="P5" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>25</v>
-      </c>
-      <c r="R5" t="n">
-        <v>33</v>
-      </c>
-      <c r="S5" t="n">
-        <v>24</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.5293186647539065</v>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
+        <v>0.3686933235895507</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Grow millets (sorghum, pearl millet), pulses (pigeon pea, chickpea), and oilseeds (safflower, castor).</t>
         </is>
       </c>
     </row>

</xml_diff>